<commit_message>
Pushing the working code of ACME - Work Items Process
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f8b04ab2bc622ed/Documents/GitHub/UiPath-ACME-Calculate-Client-Security-Hash/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBD01DB0-7F27-4AE5-91AF-10155CE2C2E7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -98,68 +98,82 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>WI5</t>
+  </si>
+  <si>
+    <t>Use comma (,) separator for multiple filter Types</t>
+  </si>
+  <si>
+    <t>Process_Filter_Type</t>
+  </si>
+  <si>
+    <t>ACME_Work_Item</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>ACME_Login_Credentials</t>
+  </si>
+  <si>
+    <t>ACME credentials from Asset</t>
   </si>
 </sst>
 </file>
@@ -212,10 +226,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -239,9 +253,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +293,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +399,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,10 +599,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -596,11 +610,11 @@
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -617,9 +631,29 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1673,18 +1707,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1742,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1764,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1775,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1786,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,7 +2816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2800,7 +2836,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>